<commit_message>
different way to calculate accuracy
</commit_message>
<xml_diff>
--- a/output/frat/depth_1/templates/frat_3_conceptnet_search.xlsx
+++ b/output/frat/depth_1/templates/frat_3_conceptnet_search.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rejna/projects/github.com/r_m_thesis/output/frat/depth_1/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C2F77E-C632-1948-8EDA-CA04D547958D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63509BD0-97F5-BD4C-B2BA-F4765F32D72A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -871,6 +871,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.1640625" customWidth="1"/>
     <col min="7" max="7" width="35.33203125" customWidth="1"/>

</xml_diff>